<commit_message>
add correct in code 02.05
</commit_message>
<xml_diff>
--- a/Excel/dane.xlsx
+++ b/Excel/dane.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projecty ŁączyMy\api_django\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projecty ŁączyMy\api_django\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B67E59-0910-4436-8F57-8355306BE871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCB3179-1A11-4A83-9B7E-987F7473F012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,11 +171,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -458,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +494,7 @@
     </row>
     <row r="2" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -513,7 +514,7 @@
     </row>
     <row r="3" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
@@ -533,7 +534,7 @@
     </row>
     <row r="4" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -553,7 +554,7 @@
     </row>
     <row r="5" spans="1:6" ht="255" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>18</v>
@@ -573,7 +574,7 @@
     </row>
     <row r="6" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>22</v>
@@ -593,7 +594,7 @@
     </row>
     <row r="7" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>26</v>
@@ -621,12 +622,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245E4447-D3AB-4B67-BDBE-187D0F145BFF}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -634,7 +636,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C1" t="s">
@@ -646,89 +648,90 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3.75</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4.25</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2.25</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.75</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>